<commit_message>
test data updated second time
</commit_message>
<xml_diff>
--- a/TestData/Test_Data.xlsx
+++ b/TestData/Test_Data.xlsx
@@ -3,9 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{B8924DBE-2CD4-40A0-B06A-EB1466F81FD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Selenium_WorkSpace\RestAssuredFrameWork\TestData\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F9A6AE2-F668-480D-B884-824576280FB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3510" yWindow="3510" windowWidth="29070" windowHeight="16500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Customer" sheetId="1" r:id="rId1"/>
@@ -15,7 +20,6 @@
     <sheet name="TestData" sheetId="7" r:id="rId5"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="61">
   <si>
     <t>name</t>
   </si>
@@ -189,19 +193,25 @@
     <t>updateSingleCustomer</t>
   </si>
   <si>
-    <t>cus_KHPFzl6Rge4XjS</t>
-  </si>
-  <si>
-    <t>cus_KHPFhpYfC1TpzV</t>
-  </si>
-  <si>
-    <t>cus_KHPFFr9kPB6111</t>
-  </si>
-  <si>
-    <t>cus_KHPA0HWMcTL3lI</t>
-  </si>
-  <si>
-    <t>cus_KHPAsgdzVEm61R</t>
+    <t>cus_KHPAJc1Gvehntk</t>
+  </si>
+  <si>
+    <t>cus_KHOlsXxLKlX9nS</t>
+  </si>
+  <si>
+    <t>cus_KHOldthDPbluyt</t>
+  </si>
+  <si>
+    <t>cus_KHOl86QmF04Gkg</t>
+  </si>
+  <si>
+    <t>cus_KHOfAbofEB8AAm</t>
+  </si>
+  <si>
+    <t>cus_KHOf8fZSlUWWzy</t>
+  </si>
+  <si>
+    <t>cus_KHOfRPNKXnm5rP</t>
   </si>
 </sst>
 </file>
@@ -1431,7 +1441,7 @@
   <dimension ref="A1:J31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I21" sqref="I21"/>
+      <selection activeCell="A29" sqref="A29:A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1733,9 +1743,7 @@
       <c r="I17" s="4"/>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18" s="6" t="s">
-        <v>58</v>
-      </c>
+      <c r="A18" s="6"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
       <c r="D18" s="4"/>
@@ -1828,7 +1836,7 @@
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="6" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="B29" t="s">
         <v>41</v>
@@ -1860,7 +1868,7 @@
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="6" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B30" t="s">
         <v>41</v>
@@ -1892,7 +1900,7 @@
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="6" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="B31" t="s">
         <v>41</v>

</xml_diff>